<commit_message>
la de la insconsistente.
</commit_message>
<xml_diff>
--- a/DB/Tablas de aprendizaje de movimientos/Gastly, Haunter y Gengar.xlsx
+++ b/DB/Tablas de aprendizaje de movimientos/Gastly, Haunter y Gengar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfax\Desktop\convertidas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oxikr\source\repos\monster-Feudal\DB\Tablas de aprendizaje de movimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>

</xml_diff>